<commit_message>
Met à jour le fichier "Nombre total de combinaisons.xlsx" avec de nouvelles données.
</commit_message>
<xml_diff>
--- a/Nombre total de combinaisons.xlsx
+++ b/Nombre total de combinaisons.xlsx
@@ -1,22 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SebastienGrison\Documents\GitHub\project-7-algorithms\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebast20200609165654\Documents\Visual Studio Code\project-7-algorithms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D41C5ED-0711-476D-9F6A-C0C43CE63ABB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F6A257A-367D-429B-ADF6-8D85040C2983}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9045" yWindow="4440" windowWidth="37755" windowHeight="14865" xr2:uid="{116C2F12-22C3-45F6-85FB-8CCAB39352F8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{116C2F12-22C3-45F6-85FB-8CCAB39352F8}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Liste actions" sheetId="3" r:id="rId2"/>
+    <sheet name="dp" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$I$1:$L$21</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Liste actions'!$A$1:$D$21</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="31">
   <si>
     <t>Taille</t>
   </si>
@@ -121,13 +124,23 @@
   </si>
   <si>
     <t>Benef€</t>
+  </si>
+  <si>
+    <t>N°</t>
+  </si>
+  <si>
+    <t>Nom</t>
+  </si>
+  <si>
+    <t>Coût</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
+    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
@@ -190,11 +203,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -208,9 +222,16 @@
     <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Milliers" xfId="1" builtinId="3"/>
+    <cellStyle name="Monétaire" xfId="2" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -227,9 +248,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office 2013 – 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -267,7 +288,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -373,7 +394,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -515,7 +536,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -525,7 +546,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{190D2F42-C245-484D-A4C9-55C3DB50AFBF}">
   <dimension ref="B1:L23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:L21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -567,7 +590,7 @@
         <v>0.13</v>
       </c>
       <c r="L2">
-        <f>J2*K2</f>
+        <f t="shared" ref="L2:L21" si="0">J2*K2</f>
         <v>6.24</v>
       </c>
     </row>
@@ -592,7 +615,7 @@
         <v>0.11</v>
       </c>
       <c r="L3">
-        <f>J3*K3</f>
+        <f t="shared" si="0"/>
         <v>2.86</v>
       </c>
     </row>
@@ -619,21 +642,21 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="L4">
-        <f>J4*K4</f>
+        <f t="shared" si="0"/>
         <v>1.54</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" s="3">
-        <f t="shared" ref="B5:B22" si="0">B4</f>
+        <f t="shared" ref="B5:B22" si="1">B4</f>
         <v>20</v>
       </c>
       <c r="C5" s="3">
-        <f t="shared" ref="C5:C22" si="1">C4+1</f>
+        <f t="shared" ref="C5:C22" si="2">C4+1</f>
         <v>3</v>
       </c>
       <c r="D5" s="4">
-        <f t="shared" ref="D5:D22" si="2">COMBIN(B5,C5)</f>
+        <f t="shared" ref="D5:D22" si="3">COMBIN(B5,C5)</f>
         <v>1140</v>
       </c>
       <c r="I5" s="5" t="s">
@@ -646,21 +669,21 @@
         <v>0.25</v>
       </c>
       <c r="L5" s="7">
-        <f>J5*K5</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="C6" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="D6" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4845</v>
       </c>
       <c r="I6" s="5" t="s">
@@ -673,21 +696,21 @@
         <v>0.17</v>
       </c>
       <c r="L6" s="7">
-        <f>J6*K6</f>
+        <f t="shared" si="0"/>
         <v>10.200000000000001</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="C7" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="D7" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>15503.999999999998</v>
       </c>
       <c r="I7" s="5" t="s">
@@ -700,21 +723,21 @@
         <v>0.2</v>
       </c>
       <c r="L7" s="7">
-        <f>J7*K7</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="C8" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="D8" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>38760</v>
       </c>
       <c r="I8" s="5" t="s">
@@ -727,21 +750,21 @@
         <v>0.15</v>
       </c>
       <c r="L8">
-        <f>J8*K8</f>
+        <f t="shared" si="0"/>
         <v>7.5</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="C9" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="D9" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>77520</v>
       </c>
       <c r="I9" s="5" t="s">
@@ -754,21 +777,21 @@
         <v>0.18</v>
       </c>
       <c r="L9" s="7">
-        <f>J9*K9</f>
+        <f t="shared" si="0"/>
         <v>20.52</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="C10" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="D10" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>125970.00000000001</v>
       </c>
       <c r="I10" s="5" t="s">
@@ -781,21 +804,21 @@
         <v>0.1</v>
       </c>
       <c r="L10" s="9">
-        <f>J10*K10</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="C11" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="D11" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>167960</v>
       </c>
       <c r="I11" s="5" t="s">
@@ -808,21 +831,21 @@
         <v>0.21</v>
       </c>
       <c r="L11" s="7">
-        <f>J11*K11</f>
+        <f t="shared" si="0"/>
         <v>5.04</v>
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="C12" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="D12" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>184756</v>
       </c>
       <c r="I12" s="5" t="s">
@@ -835,21 +858,21 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="L12">
-        <f>J12*K12</f>
+        <f t="shared" si="0"/>
         <v>1.4000000000000001</v>
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="C13" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="D13" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>167960</v>
       </c>
       <c r="I13" s="5" t="s">
@@ -862,21 +885,21 @@
         <v>0.12</v>
       </c>
       <c r="L13">
-        <f>J13*K13</f>
+        <f t="shared" si="0"/>
         <v>0.48</v>
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="C14" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="D14" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>125970.00000000001</v>
       </c>
       <c r="I14" s="5" t="s">
@@ -889,21 +912,21 @@
         <v>0.08</v>
       </c>
       <c r="L14">
-        <f>J14*K14</f>
+        <f t="shared" si="0"/>
         <v>0.64</v>
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="C15" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
       <c r="D15" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>77520</v>
       </c>
       <c r="I15" s="5" t="s">
@@ -916,21 +939,21 @@
         <v>0.03</v>
       </c>
       <c r="L15">
-        <f>J15*K15</f>
+        <f t="shared" si="0"/>
         <v>0.54</v>
       </c>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="C16" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="D16" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>38760</v>
       </c>
       <c r="I16" s="5" t="s">
@@ -943,21 +966,21 @@
         <v>0.01</v>
       </c>
       <c r="L16">
-        <f>J16*K16</f>
+        <f t="shared" si="0"/>
         <v>0.14000000000000001</v>
       </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="C17" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="D17" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>15503.999999999998</v>
       </c>
       <c r="I17" s="5" t="s">
@@ -970,21 +993,21 @@
         <v>0.23</v>
       </c>
       <c r="L17" s="7">
-        <f>J17*K17</f>
+        <f t="shared" si="0"/>
         <v>8.74</v>
       </c>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="C18" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="D18" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4845</v>
       </c>
       <c r="I18" s="5" t="s">
@@ -997,21 +1020,21 @@
         <v>0.09</v>
       </c>
       <c r="L18" s="9">
-        <f>J18*K18</f>
+        <f t="shared" si="0"/>
         <v>9.9</v>
       </c>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="C19" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>17</v>
       </c>
       <c r="D19" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1140</v>
       </c>
       <c r="I19" s="5" t="s">
@@ -1024,21 +1047,21 @@
         <v>0.17</v>
       </c>
       <c r="L19" s="7">
-        <f>J19*K19</f>
+        <f t="shared" si="0"/>
         <v>7.1400000000000006</v>
       </c>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="C20" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="D20" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>190</v>
       </c>
       <c r="I20" s="5" t="s">
@@ -1051,21 +1074,21 @@
         <v>0.27</v>
       </c>
       <c r="L20" s="7">
-        <f>J20*K20</f>
+        <f t="shared" si="0"/>
         <v>9.18</v>
       </c>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B21" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="C21" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>19</v>
       </c>
       <c r="D21" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="I21" s="5" t="s">
@@ -1078,21 +1101,21 @@
         <v>0.05</v>
       </c>
       <c r="L21">
-        <f>J21*K21</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="C22" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="D22" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -1114,4 +1137,1088 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65453F7C-0940-4BC6-89AF-5963DF981F56}">
+  <dimension ref="A1:D21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="9">
+        <v>20</v>
+      </c>
+      <c r="C2" s="10">
+        <v>0.05</v>
+      </c>
+      <c r="D2" s="12">
+        <f>B2*C2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="9">
+        <v>34</v>
+      </c>
+      <c r="C3" s="10">
+        <v>0.27</v>
+      </c>
+      <c r="D3" s="12">
+        <f>B3*C3</f>
+        <v>9.18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="9">
+        <v>42</v>
+      </c>
+      <c r="C4" s="10">
+        <v>0.17</v>
+      </c>
+      <c r="D4" s="12">
+        <f>B4*C4</f>
+        <v>7.1400000000000006</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="9">
+        <v>110</v>
+      </c>
+      <c r="C5" s="10">
+        <v>0.09</v>
+      </c>
+      <c r="D5" s="12">
+        <f>B5*C5</f>
+        <v>9.9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="9">
+        <v>38</v>
+      </c>
+      <c r="C6" s="10">
+        <v>0.23</v>
+      </c>
+      <c r="D6" s="12">
+        <f>B6*C6</f>
+        <v>8.74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="9">
+        <v>14</v>
+      </c>
+      <c r="C7" s="10">
+        <v>0.01</v>
+      </c>
+      <c r="D7" s="12">
+        <f>B7*C7</f>
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="9">
+        <v>18</v>
+      </c>
+      <c r="C8" s="10">
+        <v>0.03</v>
+      </c>
+      <c r="D8" s="12">
+        <f>B8*C8</f>
+        <v>0.54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="9">
+        <v>8</v>
+      </c>
+      <c r="C9" s="10">
+        <v>0.08</v>
+      </c>
+      <c r="D9" s="12">
+        <f>B9*C9</f>
+        <v>0.64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="9">
+        <v>4</v>
+      </c>
+      <c r="C10" s="10">
+        <v>0.12</v>
+      </c>
+      <c r="D10" s="12">
+        <f>B10*C10</f>
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="9">
+        <v>10</v>
+      </c>
+      <c r="C11" s="10">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="D11" s="12">
+        <f>B11*C11</f>
+        <v>1.4000000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="9">
+        <v>24</v>
+      </c>
+      <c r="C12" s="10">
+        <v>0.21</v>
+      </c>
+      <c r="D12" s="12">
+        <f>B12*C12</f>
+        <v>5.04</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="9">
+        <v>30</v>
+      </c>
+      <c r="C13" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="D13" s="12">
+        <f>B13*C13</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="9">
+        <v>114</v>
+      </c>
+      <c r="C14" s="10">
+        <v>0.18</v>
+      </c>
+      <c r="D14" s="12">
+        <f>B14*C14</f>
+        <v>20.52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="9">
+        <v>50</v>
+      </c>
+      <c r="C15" s="10">
+        <v>0.15</v>
+      </c>
+      <c r="D15" s="12">
+        <f>B15*C15</f>
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="9">
+        <v>70</v>
+      </c>
+      <c r="C16" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="D16" s="12">
+        <f>B16*C16</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="9">
+        <v>60</v>
+      </c>
+      <c r="C17" s="10">
+        <v>0.17</v>
+      </c>
+      <c r="D17" s="12">
+        <f>B17*C17</f>
+        <v>10.200000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="9">
+        <v>80</v>
+      </c>
+      <c r="C18" s="10">
+        <v>0.25</v>
+      </c>
+      <c r="D18" s="12">
+        <f>B18*C18</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="9">
+        <v>22</v>
+      </c>
+      <c r="C19" s="10">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D19" s="12">
+        <f>B19*C19</f>
+        <v>1.54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" s="9">
+        <v>26</v>
+      </c>
+      <c r="C20" s="10">
+        <v>0.11</v>
+      </c>
+      <c r="D20" s="12">
+        <f>B20*C20</f>
+        <v>2.86</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" s="9">
+        <v>48</v>
+      </c>
+      <c r="C21" s="10">
+        <v>0.13</v>
+      </c>
+      <c r="D21" s="12">
+        <f>B21*C21</f>
+        <v>6.24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C69D48BF-2688-400F-81B0-5028750C6D87}">
+  <dimension ref="A1:CP21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="5.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="13" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="94" width="8.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:94" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="14">
+        <v>1</v>
+      </c>
+      <c r="F1" s="14">
+        <f>E1+1</f>
+        <v>2</v>
+      </c>
+      <c r="G1" s="14">
+        <f>F1+1</f>
+        <v>3</v>
+      </c>
+      <c r="H1" s="14">
+        <f>G1+1</f>
+        <v>4</v>
+      </c>
+      <c r="I1" s="14">
+        <f>H1+1</f>
+        <v>5</v>
+      </c>
+      <c r="J1" s="14">
+        <f t="shared" ref="J1:BU1" si="0">I1+1</f>
+        <v>6</v>
+      </c>
+      <c r="K1" s="14">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="L1" s="14">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="M1" s="14">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="N1" s="14">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="O1" s="14">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="P1" s="14">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="Q1" s="14">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="R1" s="14">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="S1" s="14">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="T1" s="14">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="U1" s="14">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="V1" s="14">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="W1" s="14">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="X1" s="14">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="Y1" s="14">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="Z1" s="14">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="AA1" s="14">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="AB1" s="14">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="AC1" s="14">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="AD1" s="14">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="AE1" s="14">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="AF1" s="14">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="AG1" s="14">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="AH1" s="14">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="AI1" s="14">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="AJ1" s="14">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="AK1" s="14">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="AL1" s="14">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="AM1" s="14">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="AN1" s="14">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="AO1" s="14">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="AP1" s="14">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="AQ1" s="14">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="AR1" s="14">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="AS1" s="14">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="AT1" s="14">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="AU1" s="14">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="AV1" s="14">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="AW1" s="14">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="AX1" s="14">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="AY1" s="14">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="AZ1" s="14">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="BA1" s="14">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="BB1" s="14">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="BC1" s="14">
+        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
+      <c r="BD1" s="14">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="BE1" s="14">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
+      <c r="BF1" s="14">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="BG1" s="14">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+      <c r="BH1" s="14">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="BI1" s="14">
+        <f t="shared" si="0"/>
+        <v>57</v>
+      </c>
+      <c r="BJ1" s="14">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="BK1" s="14">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
+      <c r="BL1" s="14">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="BM1" s="14">
+        <f t="shared" si="0"/>
+        <v>61</v>
+      </c>
+      <c r="BN1" s="14">
+        <f t="shared" si="0"/>
+        <v>62</v>
+      </c>
+      <c r="BO1" s="14">
+        <f t="shared" si="0"/>
+        <v>63</v>
+      </c>
+      <c r="BP1" s="14">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="BQ1" s="14">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+      <c r="BR1" s="14">
+        <f t="shared" si="0"/>
+        <v>66</v>
+      </c>
+      <c r="BS1" s="14">
+        <f t="shared" si="0"/>
+        <v>67</v>
+      </c>
+      <c r="BT1" s="14">
+        <f t="shared" si="0"/>
+        <v>68</v>
+      </c>
+      <c r="BU1" s="14">
+        <f t="shared" si="0"/>
+        <v>69</v>
+      </c>
+      <c r="BV1" s="14">
+        <f t="shared" ref="BV1:CP1" si="1">BU1+1</f>
+        <v>70</v>
+      </c>
+      <c r="BW1" s="14">
+        <f t="shared" si="1"/>
+        <v>71</v>
+      </c>
+      <c r="BX1" s="14">
+        <f t="shared" si="1"/>
+        <v>72</v>
+      </c>
+      <c r="BY1" s="14">
+        <f t="shared" si="1"/>
+        <v>73</v>
+      </c>
+      <c r="BZ1" s="14">
+        <f t="shared" si="1"/>
+        <v>74</v>
+      </c>
+      <c r="CA1" s="14">
+        <f t="shared" si="1"/>
+        <v>75</v>
+      </c>
+      <c r="CB1" s="14">
+        <f t="shared" si="1"/>
+        <v>76</v>
+      </c>
+      <c r="CC1" s="14">
+        <f t="shared" si="1"/>
+        <v>77</v>
+      </c>
+      <c r="CD1" s="14">
+        <f t="shared" si="1"/>
+        <v>78</v>
+      </c>
+      <c r="CE1" s="14">
+        <f t="shared" si="1"/>
+        <v>79</v>
+      </c>
+      <c r="CF1" s="14">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+      <c r="CG1" s="14">
+        <f t="shared" si="1"/>
+        <v>81</v>
+      </c>
+      <c r="CH1" s="14">
+        <f t="shared" si="1"/>
+        <v>82</v>
+      </c>
+      <c r="CI1" s="14">
+        <f t="shared" si="1"/>
+        <v>83</v>
+      </c>
+      <c r="CJ1" s="14">
+        <f t="shared" si="1"/>
+        <v>84</v>
+      </c>
+      <c r="CK1" s="14">
+        <f t="shared" si="1"/>
+        <v>85</v>
+      </c>
+      <c r="CL1" s="14">
+        <f t="shared" si="1"/>
+        <v>86</v>
+      </c>
+      <c r="CM1" s="14">
+        <f t="shared" si="1"/>
+        <v>87</v>
+      </c>
+      <c r="CN1" s="14">
+        <f t="shared" si="1"/>
+        <v>88</v>
+      </c>
+      <c r="CO1" s="14">
+        <f t="shared" si="1"/>
+        <v>89</v>
+      </c>
+      <c r="CP1" s="14">
+        <f t="shared" si="1"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:94" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="11" t="str">
+        <f>"Action-"&amp;A2</f>
+        <v>Action-1</v>
+      </c>
+      <c r="C2" s="11">
+        <f>INDEX('Liste actions'!B:B,MATCH(dp!B2,'Liste actions'!A:A,0))</f>
+        <v>20</v>
+      </c>
+      <c r="D2" s="11">
+        <f>INDEX('Liste actions'!D:D,MATCH(dp!B2,'Liste actions'!A:A,0))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:94" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f>A2+1</f>
+        <v>2</v>
+      </c>
+      <c r="B3" s="11" t="str">
+        <f t="shared" ref="B3:B21" si="2">"Action-"&amp;A3</f>
+        <v>Action-2</v>
+      </c>
+      <c r="C3" s="11">
+        <f>INDEX('Liste actions'!B:B,MATCH(dp!B3,'Liste actions'!A:A,0))</f>
+        <v>30</v>
+      </c>
+      <c r="D3" s="11">
+        <f>INDEX('Liste actions'!D:D,MATCH(dp!B3,'Liste actions'!A:A,0))</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:94" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f t="shared" ref="A4:A21" si="3">A3+1</f>
+        <v>3</v>
+      </c>
+      <c r="B4" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>Action-3</v>
+      </c>
+      <c r="C4" s="11">
+        <f>INDEX('Liste actions'!B:B,MATCH(dp!B4,'Liste actions'!A:A,0))</f>
+        <v>50</v>
+      </c>
+      <c r="D4" s="11">
+        <f>INDEX('Liste actions'!D:D,MATCH(dp!B4,'Liste actions'!A:A,0))</f>
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:94" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="B5" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>Action-4</v>
+      </c>
+      <c r="C5" s="11">
+        <f>INDEX('Liste actions'!B:B,MATCH(dp!B5,'Liste actions'!A:A,0))</f>
+        <v>70</v>
+      </c>
+      <c r="D5" s="11">
+        <f>INDEX('Liste actions'!D:D,MATCH(dp!B5,'Liste actions'!A:A,0))</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:94" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="B6" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>Action-5</v>
+      </c>
+      <c r="C6" s="11">
+        <f>INDEX('Liste actions'!B:B,MATCH(dp!B6,'Liste actions'!A:A,0))</f>
+        <v>60</v>
+      </c>
+      <c r="D6" s="11">
+        <f>INDEX('Liste actions'!D:D,MATCH(dp!B6,'Liste actions'!A:A,0))</f>
+        <v>10.200000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:94" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="B7" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>Action-6</v>
+      </c>
+      <c r="C7" s="11">
+        <f>INDEX('Liste actions'!B:B,MATCH(dp!B7,'Liste actions'!A:A,0))</f>
+        <v>80</v>
+      </c>
+      <c r="D7" s="11">
+        <f>INDEX('Liste actions'!D:D,MATCH(dp!B7,'Liste actions'!A:A,0))</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:94" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="B8" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>Action-7</v>
+      </c>
+      <c r="C8" s="11">
+        <f>INDEX('Liste actions'!B:B,MATCH(dp!B8,'Liste actions'!A:A,0))</f>
+        <v>22</v>
+      </c>
+      <c r="D8" s="11">
+        <f>INDEX('Liste actions'!D:D,MATCH(dp!B8,'Liste actions'!A:A,0))</f>
+        <v>1.54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:94" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="B9" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>Action-8</v>
+      </c>
+      <c r="C9" s="11">
+        <f>INDEX('Liste actions'!B:B,MATCH(dp!B9,'Liste actions'!A:A,0))</f>
+        <v>26</v>
+      </c>
+      <c r="D9" s="11">
+        <f>INDEX('Liste actions'!D:D,MATCH(dp!B9,'Liste actions'!A:A,0))</f>
+        <v>2.86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:94" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="B10" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>Action-9</v>
+      </c>
+      <c r="C10" s="11">
+        <f>INDEX('Liste actions'!B:B,MATCH(dp!B10,'Liste actions'!A:A,0))</f>
+        <v>48</v>
+      </c>
+      <c r="D10" s="11">
+        <f>INDEX('Liste actions'!D:D,MATCH(dp!B10,'Liste actions'!A:A,0))</f>
+        <v>6.24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:94" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="B11" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>Action-10</v>
+      </c>
+      <c r="C11" s="11">
+        <f>INDEX('Liste actions'!B:B,MATCH(dp!B11,'Liste actions'!A:A,0))</f>
+        <v>34</v>
+      </c>
+      <c r="D11" s="11">
+        <f>INDEX('Liste actions'!D:D,MATCH(dp!B11,'Liste actions'!A:A,0))</f>
+        <v>9.18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:94" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f t="shared" si="3"/>
+        <v>11</v>
+      </c>
+      <c r="B12" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>Action-11</v>
+      </c>
+      <c r="C12" s="11">
+        <f>INDEX('Liste actions'!B:B,MATCH(dp!B12,'Liste actions'!A:A,0))</f>
+        <v>42</v>
+      </c>
+      <c r="D12" s="11">
+        <f>INDEX('Liste actions'!D:D,MATCH(dp!B12,'Liste actions'!A:A,0))</f>
+        <v>7.1400000000000006</v>
+      </c>
+    </row>
+    <row r="13" spans="1:94" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+      <c r="B13" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>Action-12</v>
+      </c>
+      <c r="C13" s="11">
+        <f>INDEX('Liste actions'!B:B,MATCH(dp!B13,'Liste actions'!A:A,0))</f>
+        <v>110</v>
+      </c>
+      <c r="D13" s="11">
+        <f>INDEX('Liste actions'!D:D,MATCH(dp!B13,'Liste actions'!A:A,0))</f>
+        <v>9.9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:94" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f t="shared" si="3"/>
+        <v>13</v>
+      </c>
+      <c r="B14" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>Action-13</v>
+      </c>
+      <c r="C14" s="11">
+        <f>INDEX('Liste actions'!B:B,MATCH(dp!B14,'Liste actions'!A:A,0))</f>
+        <v>38</v>
+      </c>
+      <c r="D14" s="11">
+        <f>INDEX('Liste actions'!D:D,MATCH(dp!B14,'Liste actions'!A:A,0))</f>
+        <v>8.74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:94" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+      <c r="B15" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>Action-14</v>
+      </c>
+      <c r="C15" s="11">
+        <f>INDEX('Liste actions'!B:B,MATCH(dp!B15,'Liste actions'!A:A,0))</f>
+        <v>14</v>
+      </c>
+      <c r="D15" s="11">
+        <f>INDEX('Liste actions'!D:D,MATCH(dp!B15,'Liste actions'!A:A,0))</f>
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:94" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+      <c r="B16" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>Action-15</v>
+      </c>
+      <c r="C16" s="11">
+        <f>INDEX('Liste actions'!B:B,MATCH(dp!B16,'Liste actions'!A:A,0))</f>
+        <v>18</v>
+      </c>
+      <c r="D16" s="11">
+        <f>INDEX('Liste actions'!D:D,MATCH(dp!B16,'Liste actions'!A:A,0))</f>
+        <v>0.54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+      <c r="B17" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>Action-16</v>
+      </c>
+      <c r="C17" s="11">
+        <f>INDEX('Liste actions'!B:B,MATCH(dp!B17,'Liste actions'!A:A,0))</f>
+        <v>8</v>
+      </c>
+      <c r="D17" s="11">
+        <f>INDEX('Liste actions'!D:D,MATCH(dp!B17,'Liste actions'!A:A,0))</f>
+        <v>0.64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <f t="shared" si="3"/>
+        <v>17</v>
+      </c>
+      <c r="B18" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>Action-17</v>
+      </c>
+      <c r="C18" s="11">
+        <f>INDEX('Liste actions'!B:B,MATCH(dp!B18,'Liste actions'!A:A,0))</f>
+        <v>4</v>
+      </c>
+      <c r="D18" s="11">
+        <f>INDEX('Liste actions'!D:D,MATCH(dp!B18,'Liste actions'!A:A,0))</f>
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <f t="shared" si="3"/>
+        <v>18</v>
+      </c>
+      <c r="B19" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>Action-18</v>
+      </c>
+      <c r="C19" s="11">
+        <f>INDEX('Liste actions'!B:B,MATCH(dp!B19,'Liste actions'!A:A,0))</f>
+        <v>10</v>
+      </c>
+      <c r="D19" s="11">
+        <f>INDEX('Liste actions'!D:D,MATCH(dp!B19,'Liste actions'!A:A,0))</f>
+        <v>1.4000000000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <f t="shared" si="3"/>
+        <v>19</v>
+      </c>
+      <c r="B20" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>Action-19</v>
+      </c>
+      <c r="C20" s="11">
+        <f>INDEX('Liste actions'!B:B,MATCH(dp!B20,'Liste actions'!A:A,0))</f>
+        <v>24</v>
+      </c>
+      <c r="D20" s="11">
+        <f>INDEX('Liste actions'!D:D,MATCH(dp!B20,'Liste actions'!A:A,0))</f>
+        <v>5.04</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="B21" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>Action-20</v>
+      </c>
+      <c r="C21" s="11">
+        <f>INDEX('Liste actions'!B:B,MATCH(dp!B21,'Liste actions'!A:A,0))</f>
+        <v>114</v>
+      </c>
+      <c r="D21" s="11">
+        <f>INDEX('Liste actions'!D:D,MATCH(dp!B21,'Liste actions'!A:A,0))</f>
+        <v>20.52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>